<commit_message>
fix(): Updated Excel templates
</commit_message>
<xml_diff>
--- a/default-mappings-xlsx/grabber/Grabber_Mapping_Hubspot_DE.xlsx
+++ b/default-mappings-xlsx/grabber/Grabber_Mapping_Hubspot_DE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSchönrock\Documents\Neue Vorlagen\Grabber\Hubspot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSchönrock\Documents\Neue Vorlagen\Export Ready\grabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D7AA0-ADA3-40D1-A105-16FD70F15FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98A407-21A9-41FD-9C7E-2C4E486FB079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4740A9B0-2E57-42FE-A57B-C2BAD0638104}"/>
   </bookViews>
@@ -34,6 +34,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Valentin Schönrock</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{6BB13B31-BB63-41BC-A3B7-87A32439B3C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>"x" eingeben, wenn dieses Feld ausgefüllt sein muss</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{7D083F8D-F203-4ED3-9A3D-DBF149D94168}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>"x" eingeben, wenn dieses Feld nicht benötigt wird</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
@@ -212,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +325,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1913,12 +1958,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795B0A9E-16D1-4F4A-842C-C5B0396BE825}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795B0A9E-16D1-4F4A-842C-C5B0396BE825}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:CI31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,15 +2719,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q20:Q30 I20:I30 I7:I17 Q7:Q17 M20:M30 M7:M17" xr:uid="{5EC9FB2D-F3B3-4F68-88B9-BC7DBE621DBB}">
-      <formula1>"text,picklist,multi-picklist,lookup,date,number"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D17" xr:uid="{2F7FE776-7F87-432C-9F15-37A73F22AC1A}">
       <formula1>"x"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I17 M7:M17 Q7:Q17 Q20:Q30 M20:M30 I20:I30" xr:uid="{6497D81A-C6CE-4DCD-9058-213762C32894}">
+      <formula1>"text,picklist,multi-picklist,lookup,date,number,boolean"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(): Hubspot Excel templates
</commit_message>
<xml_diff>
--- a/default-mappings-xlsx/grabber/Grabber_Mapping_Hubspot_DE.xlsx
+++ b/default-mappings-xlsx/grabber/Grabber_Mapping_Hubspot_DE.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSchönrock\Documents\GitRepos\snapaddy-faq-attachments\default-mappings-xlsx\grabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22625A5-8D20-4825-8EBF-28FA5782F063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD20E6-8E02-4E19-B4E4-C0E1C938E23A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="2565" windowWidth="5445" windowHeight="12210" xr2:uid="{4740A9B0-2E57-42FE-A57B-C2BAD0638104}"/>
+    <workbookView xWindow="30960" yWindow="2400" windowWidth="14460" windowHeight="15600" xr2:uid="{4740A9B0-2E57-42FE-A57B-C2BAD0638104}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Checkbox">Tabelle1!$C$7:$C$17</definedName>
-    <definedName name="Field_Type">Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!$P$7:$P$17,Tabelle1!$P$20:$P$30,Tabelle1!$H$20:$H$30,Tabelle1!$H$7:$H$17</definedName>
+    <definedName name="Checkbox">Tabelle1!$C$7:$C$25</definedName>
+    <definedName name="Field_Type">Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!#REF!,Tabelle1!$P$7:$P$25,Tabelle1!$P$28:$P$38,Tabelle1!$H$28:$H$38,Tabelle1!$H$7:$H$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
   <si>
     <t>snapADDY</t>
   </si>
@@ -118,12 +118,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>Pipeline-Phase</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -197,6 +191,60 @@
   </si>
   <si>
     <t>Grabber Mapping</t>
+  </si>
+  <si>
+    <t>Anrede</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>MobilTelefon</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>jobtitle</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>mobilephone</t>
+  </si>
+  <si>
+    <t>picklist</t>
+  </si>
+  <si>
+    <t>domain</t>
   </si>
 </sst>
 </file>
@@ -312,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -967,11 +1015,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9DA600"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF9DA600"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF9DA600"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFF87757"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF87757"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF87757"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFF87757"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF87757"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1069,9 +1161,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1090,11 +1179,306 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1264,13 +1648,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>973015</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>105510</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>4396</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1335,13 +1719,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>973015</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>105510</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>4396</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1703,9 +2087,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795B0A9E-16D1-4F4A-842C-C5B0396BE825}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:CH31"/>
+  <dimension ref="A1:CH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1724,7 +2110,7 @@
   <sheetData>
     <row r="1" spans="1:86" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1746,26 +2132,26 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="F4" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="F4" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
+      <c r="N4" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
     </row>
     <row r="5" spans="1:86" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:86" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1821,172 +2207,100 @@
       <c r="P7" s="50"/>
     </row>
     <row r="8" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="J8" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="53"/>
+      <c r="A8" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="14"/>
+      <c r="F8" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="69"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="69"/>
     </row>
     <row r="9" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
-      <c r="J9" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="53"/>
-    </row>
-    <row r="10" spans="1:86" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
-      <c r="I10"/>
-      <c r="J10" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="53"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
-      <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10"/>
-      <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
-      <c r="AZ10"/>
-      <c r="BA10"/>
-      <c r="BB10"/>
-      <c r="BC10"/>
-      <c r="BD10"/>
-      <c r="BE10"/>
-      <c r="BF10"/>
-      <c r="BG10"/>
-      <c r="BH10"/>
-      <c r="BI10"/>
-      <c r="BJ10"/>
-      <c r="BK10"/>
-      <c r="BL10"/>
-      <c r="BM10"/>
-      <c r="BN10"/>
-      <c r="BO10"/>
-      <c r="BP10"/>
-      <c r="BQ10"/>
-      <c r="BR10"/>
-      <c r="BS10"/>
-      <c r="BT10"/>
-      <c r="BU10"/>
-      <c r="BV10"/>
-      <c r="BW10"/>
-      <c r="BX10"/>
-      <c r="BY10"/>
-      <c r="BZ10"/>
-      <c r="CA10"/>
-      <c r="CB10"/>
-      <c r="CC10"/>
-      <c r="CD10"/>
-      <c r="CE10"/>
-      <c r="CF10"/>
-      <c r="CG10"/>
-      <c r="CH10"/>
+      <c r="A9" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="14"/>
+      <c r="F9" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="67"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="69"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="69"/>
+    </row>
+    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="14"/>
+      <c r="F10" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="69"/>
     </row>
     <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B11" s="26"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="53"/>
-      <c r="J11" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="53"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="14"/>
+      <c r="F11" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="69"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="69"/>
     </row>
     <row r="12" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="21"/>
@@ -1995,211 +2309,326 @@
       <c r="G12" s="52"/>
       <c r="H12" s="53"/>
       <c r="J12" s="51" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K12" s="52" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L12" s="53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N12" s="51"/>
       <c r="O12" s="52"/>
       <c r="P12" s="53"/>
     </row>
     <row r="13" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="20"/>
+      <c r="A13" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="24"/>
       <c r="C13" s="21"/>
       <c r="D13" s="22"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="53"/>
+      <c r="F13" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>22</v>
+      </c>
       <c r="J13" s="51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K13" s="52" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L13" s="53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N13" s="51"/>
       <c r="O13" s="52"/>
       <c r="P13" s="53"/>
     </row>
-    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
+    <row r="14" spans="1:86" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="F14" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14"/>
       <c r="J14" s="51" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="K14" s="52" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L14" s="53" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="M14"/>
       <c r="N14" s="51"/>
       <c r="O14" s="52"/>
       <c r="P14" s="53"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14"/>
+      <c r="BH14"/>
+      <c r="BI14"/>
+      <c r="BJ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BM14"/>
+      <c r="BN14"/>
+      <c r="BO14"/>
+      <c r="BP14"/>
+      <c r="BQ14"/>
+      <c r="BR14"/>
+      <c r="BS14"/>
+      <c r="BT14"/>
+      <c r="BU14"/>
+      <c r="BV14"/>
+      <c r="BW14"/>
+      <c r="BX14"/>
+      <c r="BY14"/>
+      <c r="BZ14"/>
+      <c r="CA14"/>
+      <c r="CB14"/>
+      <c r="CC14"/>
+      <c r="CD14"/>
+      <c r="CE14"/>
+      <c r="CF14"/>
+      <c r="CG14"/>
+      <c r="CH14"/>
     </row>
     <row r="15" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="20"/>
+      <c r="A15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="26"/>
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="53"/>
-      <c r="N15" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="P15" s="53" t="s">
-        <v>24</v>
-      </c>
+      <c r="F15" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="51"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="53"/>
     </row>
     <row r="16" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="53"/>
-      <c r="N16" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="O16" s="52" t="s">
+      <c r="A16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="F16" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="56"/>
-      <c r="N17" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="O17" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="P17" s="56" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="J18" s="33"/>
-      <c r="L18" s="34"/>
-      <c r="N18" s="33"/>
-      <c r="P18" s="34"/>
-    </row>
-    <row r="19" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="N19" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="P19" s="44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="37"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="50"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="50"/>
+      <c r="J16" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="51"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="53"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="F17" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="51"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="53"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="F18" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="51"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="53"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="F19" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="53"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="53"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
+      <c r="F20" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="53"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="53"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="39"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
+      <c r="A21" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="F21" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>22</v>
+      </c>
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
       <c r="L21" s="53"/>
@@ -2208,122 +2637,171 @@
       <c r="P21" s="53"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="39"/>
+      <c r="A22" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
       <c r="F22" s="51"/>
       <c r="G22" s="52"/>
       <c r="H22" s="53"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="53"/>
+      <c r="J22" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" s="53" t="s">
+        <v>22</v>
+      </c>
       <c r="N22" s="51"/>
       <c r="O22" s="52"/>
       <c r="P22" s="53"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="39"/>
+      <c r="A23" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
       <c r="F23" s="51"/>
       <c r="G23" s="52"/>
       <c r="H23" s="53"/>
       <c r="J23" s="51"/>
       <c r="K23" s="52"/>
       <c r="L23" s="53"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="53"/>
+      <c r="N23" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="53" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="39"/>
+      <c r="A24" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
       <c r="F24" s="51"/>
       <c r="G24" s="52"/>
       <c r="H24" s="53"/>
       <c r="J24" s="51"/>
       <c r="K24" s="52"/>
       <c r="L24" s="53"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="53"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="39"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="53"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="53"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="53"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="39"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="53"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="53"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="53"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="39"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="53"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="53"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="53"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="39"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="53"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="53"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="53"/>
+      <c r="N24" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="P24" s="53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="56"/>
+      <c r="N25" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="33"/>
+      <c r="H26" s="34"/>
+      <c r="J26" s="33"/>
+      <c r="L26" s="34"/>
+      <c r="N26" s="33"/>
+      <c r="P26" s="34"/>
+    </row>
+    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="N27" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="64"/>
+      <c r="D28" s="37"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="50"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="50"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="50"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="60"/>
       <c r="D29" s="39"/>
       <c r="F29" s="51"/>
       <c r="G29" s="52"/>
@@ -2335,74 +2813,282 @@
       <c r="O29" s="52"/>
       <c r="P29" s="53"/>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="41"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="56"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="56"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="56"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="60"/>
+      <c r="D30" s="39"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="53"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="53"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="53"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="60"/>
+      <c r="D31" s="39"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="53"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="53"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="53"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="38"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="39"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="53"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="53"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="38"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="39"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="53"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="39"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="53"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="53"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="39"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="53"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="53"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="39"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="53"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="53"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="39"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="53"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="53"/>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="40"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="41"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="56"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="56"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="56"/>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A7:Q17" name="Contact Fields"/>
-    <protectedRange sqref="E20:I24 J20:Q30 C25:I30 A25:B30" name="Questionnaire"/>
+    <protectedRange sqref="A7:Q25" name="Contact Fields"/>
+    <protectedRange sqref="E28:I32 J28:Q38 A33:I38" name="Questionnaire"/>
     <protectedRange sqref="A1" name="Titel"/>
-    <protectedRange sqref="C20:D24 A20:B24" name="Questionnaire_1"/>
+    <protectedRange sqref="A28:D32" name="Questionnaire_1"/>
   </protectedRanges>
   <mergeCells count="14">
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B33:C33"/>
   </mergeCells>
-  <conditionalFormatting sqref="A17:I18 B8:I16 J8:Y18">
-    <cfRule type="expression" dxfId="5" priority="27">
+  <conditionalFormatting sqref="A25:I26 B12:Y17 B22:I24 B18:E21 G18:I21 J19:Y26 M18:Y18">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>#REF!="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="28">
+    <cfRule type="expression" dxfId="30" priority="50">
+      <formula>$C12="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28:P38 F28:H38 J28:L38">
+    <cfRule type="expression" dxfId="29" priority="63">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="64">
+      <formula>$C28="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:A24">
+    <cfRule type="expression" dxfId="27" priority="67">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="68">
+      <formula>$C12="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="20">
+      <formula>$C18="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>$C19="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>$C20="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>$C21="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18:L18">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>$C18="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>$C18="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$C8="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:P30 F20:H30 J20:L30">
-    <cfRule type="expression" dxfId="3" priority="41">
+  <conditionalFormatting sqref="F9">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>#REF!="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="42">
-      <formula>$C20="x"</formula>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$C9="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A16">
-    <cfRule type="expression" dxfId="1" priority="45">
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>#REF!="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="46">
-      <formula>$C8="x"</formula>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$C10="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>#REF!="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$C11="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H17 L7:L17 P7:P17 P20:P30 L20:L30 H20:H30" xr:uid="{6497D81A-C6CE-4DCD-9058-213762C32894}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H25 H28:H38 P7:P25 P28:P38 L28:L38 L7:L25" xr:uid="{6497D81A-C6CE-4DCD-9058-213762C32894}">
       <formula1>"text,picklist,multi-picklist,lookup,date,number,boolean"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C17" xr:uid="{2F7FE776-7F87-432C-9F15-37A73F22AC1A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C25" xr:uid="{2F7FE776-7F87-432C-9F15-37A73F22AC1A}">
       <formula1>"x"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>